<commit_message>
Updated month totals (multiplied by days)
</commit_message>
<xml_diff>
--- a/clean_avocado_data.xlsx
+++ b/clean_avocado_data.xlsx
@@ -123,29 +123,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -392,7 +386,7 @@
         <v>1.0825</v>
       </c>
       <c r="D2" s="1">
-        <v>3096334.445</v>
+        <v>9.5986367795E7</v>
       </c>
       <c r="E2" s="2">
         <v>42005.0</v>
@@ -412,7 +406,7 @@
         <v>1.18</v>
       </c>
       <c r="D3" s="1">
-        <v>192838.3025</v>
+        <v>5977987.3775</v>
       </c>
       <c r="E3" s="2">
         <v>42005.0</v>
@@ -432,7 +426,7 @@
         <v>1.295</v>
       </c>
       <c r="D4" s="1">
-        <v>258809.6125</v>
+        <v>8023097.9875</v>
       </c>
       <c r="E4" s="2">
         <v>42005.0</v>
@@ -452,7 +446,7 @@
         <v>0.7575</v>
       </c>
       <c r="D5" s="1">
-        <v>1031706.8425</v>
+        <v>3.19829121175E7</v>
       </c>
       <c r="E5" s="2">
         <v>42005.0</v>
@@ -472,7 +466,7 @@
         <v>1.1175</v>
       </c>
       <c r="D6" s="1">
-        <v>149385.2</v>
+        <v>4630941.2</v>
       </c>
       <c r="E6" s="2">
         <v>42005.0</v>
@@ -492,7 +486,7 @@
         <v>1.16</v>
       </c>
       <c r="D7" s="1">
-        <v>115675.18</v>
+        <v>3585930.58</v>
       </c>
       <c r="E7" s="2">
         <v>42005.0</v>
@@ -512,7 +506,7 @@
         <v>0.9625</v>
       </c>
       <c r="D8" s="1">
-        <v>268759.7275</v>
+        <v>8331551.5525</v>
       </c>
       <c r="E8" s="2">
         <v>42005.0</v>
@@ -532,7 +526,7 @@
         <v>0.8875</v>
       </c>
       <c r="D9" s="1">
-        <v>2631631.585</v>
+        <v>8.1580579135E7</v>
       </c>
       <c r="E9" s="2">
         <v>42005.0</v>
@@ -552,7 +546,7 @@
         <v>1.0125</v>
       </c>
       <c r="D10" s="1">
-        <v>87126.96</v>
+        <v>2700935.76</v>
       </c>
       <c r="E10" s="2">
         <v>42005.0</v>
@@ -572,7 +566,7 @@
         <v>1.205</v>
       </c>
       <c r="D11" s="1">
-        <v>421556.2775</v>
+        <v>1.30682446025E7</v>
       </c>
       <c r="E11" s="2">
         <v>42005.0</v>
@@ -592,7 +586,7 @@
         <v>1.055</v>
       </c>
       <c r="D12" s="1">
-        <v>149078.765</v>
+        <v>4621441.715</v>
       </c>
       <c r="E12" s="2">
         <v>42005.0</v>
@@ -612,7 +606,7 @@
         <v>0.97</v>
       </c>
       <c r="D13" s="1">
-        <v>250274.51</v>
+        <v>7758509.81</v>
       </c>
       <c r="E13" s="2">
         <v>42005.0</v>
@@ -632,7 +626,7 @@
         <v>1.29</v>
       </c>
       <c r="D14" s="1">
-        <v>1142066.215</v>
+        <v>3.5404052665E7</v>
       </c>
       <c r="E14" s="2">
         <v>42005.0</v>
@@ -652,7 +646,7 @@
         <v>1.24</v>
       </c>
       <c r="D15" s="1">
-        <v>3280149.725</v>
+        <v>1.01684641475E8</v>
       </c>
       <c r="E15" s="2">
         <v>42005.0</v>
@@ -672,7 +666,7 @@
         <v>1.0725</v>
       </c>
       <c r="D16" s="1">
-        <v>309088.705</v>
+        <v>9581749.855</v>
       </c>
       <c r="E16" s="2">
         <v>42005.0</v>
@@ -692,7 +686,7 @@
         <v>1.6475</v>
       </c>
       <c r="D17" s="1">
-        <v>59307.5425</v>
+        <v>1838533.8175</v>
       </c>
       <c r="E17" s="2">
         <v>42005.0</v>
@@ -712,7 +706,7 @@
         <v>1.7675</v>
       </c>
       <c r="D18" s="1">
-        <v>2576.7525</v>
+        <v>79879.3275</v>
       </c>
       <c r="E18" s="2">
         <v>42005.0</v>
@@ -732,7 +726,7 @@
         <v>2.29</v>
       </c>
       <c r="D19" s="1">
-        <v>3184.2475</v>
+        <v>98711.6725</v>
       </c>
       <c r="E19" s="2">
         <v>42005.0</v>
@@ -752,7 +746,7 @@
         <v>1.23</v>
       </c>
       <c r="D20" s="1">
-        <v>9469.4675</v>
+        <v>293553.4925</v>
       </c>
       <c r="E20" s="2">
         <v>42005.0</v>
@@ -772,7 +766,7 @@
         <v>1.8</v>
       </c>
       <c r="D21" s="1">
-        <v>1373.9875</v>
+        <v>42593.6125</v>
       </c>
       <c r="E21" s="2">
         <v>42005.0</v>
@@ -792,7 +786,7 @@
         <v>1.855</v>
       </c>
       <c r="D22" s="1">
-        <v>1293.405</v>
+        <v>40095.555</v>
       </c>
       <c r="E22" s="2">
         <v>42005.0</v>
@@ -812,7 +806,7 @@
         <v>1.5825</v>
       </c>
       <c r="D23" s="1">
-        <v>6066.3425</v>
+        <v>188056.6175</v>
       </c>
       <c r="E23" s="2">
         <v>42005.0</v>
@@ -832,7 +826,7 @@
         <v>1.2125</v>
       </c>
       <c r="D24" s="1">
-        <v>49113.84</v>
+        <v>1522529.04</v>
       </c>
       <c r="E24" s="2">
         <v>42005.0</v>
@@ -852,7 +846,7 @@
         <v>1.685</v>
       </c>
       <c r="D25" s="1">
-        <v>1284.8875</v>
+        <v>39831.5125</v>
       </c>
       <c r="E25" s="2">
         <v>42005.0</v>
@@ -872,7 +866,7 @@
         <v>1.845</v>
       </c>
       <c r="D26" s="1">
-        <v>1752.8025</v>
+        <v>54336.8775</v>
       </c>
       <c r="E26" s="2">
         <v>42005.0</v>
@@ -892,7 +886,7 @@
         <v>1.82</v>
       </c>
       <c r="D27" s="1">
-        <v>3606.4375</v>
+        <v>111799.5625</v>
       </c>
       <c r="E27" s="2">
         <v>42005.0</v>
@@ -912,7 +906,7 @@
         <v>1.325</v>
       </c>
       <c r="D28" s="1">
-        <v>2528.5</v>
+        <v>78383.5</v>
       </c>
       <c r="E28" s="2">
         <v>42005.0</v>
@@ -932,7 +926,7 @@
         <v>2.015</v>
       </c>
       <c r="D29" s="1">
-        <v>13922.0775</v>
+        <v>431584.4025</v>
       </c>
       <c r="E29" s="2">
         <v>42005.0</v>
@@ -952,7 +946,7 @@
         <v>1.9</v>
       </c>
       <c r="D30" s="1">
-        <v>43505.715</v>
+        <v>1348677.165</v>
       </c>
       <c r="E30" s="2">
         <v>42005.0</v>
@@ -972,7 +966,7 @@
         <v>1.8725</v>
       </c>
       <c r="D31" s="1">
-        <v>7040.725</v>
+        <v>218262.475</v>
       </c>
       <c r="E31" s="2">
         <v>42005.0</v>
@@ -992,7 +986,7 @@
         <v>1.0725</v>
       </c>
       <c r="D32" s="1">
-        <v>3267702.3</v>
+        <v>9.14956644E7</v>
       </c>
       <c r="E32" s="2">
         <v>42036.0</v>
@@ -1012,12 +1006,12 @@
         <v>1.125</v>
       </c>
       <c r="D33" s="1">
-        <v>225401.615</v>
+        <v>6311245.22</v>
       </c>
       <c r="E33" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1032,12 +1026,12 @@
         <v>1.295</v>
       </c>
       <c r="D34" s="1">
-        <v>276480.3775</v>
+        <v>7741450.57</v>
       </c>
       <c r="E34" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1052,12 +1046,12 @@
         <v>0.7425</v>
       </c>
       <c r="D35" s="1">
-        <v>1125570.6225</v>
+        <v>3.151597743E7</v>
       </c>
       <c r="E35" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1072,12 +1066,12 @@
         <v>1.135</v>
       </c>
       <c r="D36" s="1">
-        <v>163353.36</v>
+        <v>4573894.08</v>
       </c>
       <c r="E36" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1092,12 +1086,12 @@
         <v>1.1175</v>
       </c>
       <c r="D37" s="1">
-        <v>138994.0825</v>
+        <v>3891834.31</v>
       </c>
       <c r="E37" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1112,12 +1106,12 @@
         <v>1.0575</v>
       </c>
       <c r="D38" s="1">
-        <v>296797.84</v>
+        <v>8310339.52</v>
       </c>
       <c r="E38" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1132,12 +1126,12 @@
         <v>0.825</v>
       </c>
       <c r="D39" s="1">
-        <v>3138530.7925</v>
+        <v>8.787886219E7</v>
       </c>
       <c r="E39" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1152,12 +1146,12 @@
         <v>1.01</v>
       </c>
       <c r="D40" s="1">
-        <v>100135.03</v>
+        <v>2803780.84</v>
       </c>
       <c r="E40" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1172,12 +1166,12 @@
         <v>1.1825</v>
       </c>
       <c r="D41" s="1">
-        <v>456212.995</v>
+        <v>1.277396386E7</v>
       </c>
       <c r="E41" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1192,12 +1186,12 @@
         <v>0.99</v>
       </c>
       <c r="D42" s="1">
-        <v>173809.2475</v>
+        <v>4866658.93</v>
       </c>
       <c r="E42" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1212,12 +1206,12 @@
         <v>0.92</v>
       </c>
       <c r="D43" s="1">
-        <v>274005.1725</v>
+        <v>7672144.83</v>
       </c>
       <c r="E43" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1232,12 +1226,12 @@
         <v>1.29</v>
       </c>
       <c r="D44" s="1">
-        <v>1294752.9325</v>
+        <v>3.625308211E7</v>
       </c>
       <c r="E44" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1252,12 +1246,12 @@
         <v>1.225</v>
       </c>
       <c r="D45" s="1">
-        <v>3695518.8775</v>
+        <v>1.0347452857E8</v>
       </c>
       <c r="E45" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1272,12 +1266,12 @@
         <v>1.0825</v>
       </c>
       <c r="D46" s="1">
-        <v>332330.405</v>
+        <v>9305251.34</v>
       </c>
       <c r="E46" s="2">
         <v>42036.0</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1292,7 +1286,7 @@
         <v>1.625</v>
       </c>
       <c r="D47" s="1">
-        <v>59149.96</v>
+        <v>1656198.88</v>
       </c>
       <c r="E47" s="2">
         <v>42036.0</v>
@@ -1312,7 +1306,7 @@
         <v>1.6625</v>
       </c>
       <c r="D48" s="1">
-        <v>3826.5775</v>
+        <v>107144.17</v>
       </c>
       <c r="E48" s="2">
         <v>42036.0</v>
@@ -1332,7 +1326,7 @@
         <v>2.105</v>
       </c>
       <c r="D49" s="1">
-        <v>4724.0325</v>
+        <v>132272.91</v>
       </c>
       <c r="E49" s="2">
         <v>42036.0</v>
@@ -1352,7 +1346,7 @@
         <v>1.2375</v>
       </c>
       <c r="D50" s="1">
-        <v>10681.375</v>
+        <v>299078.5</v>
       </c>
       <c r="E50" s="2">
         <v>42036.0</v>
@@ -1372,7 +1366,7 @@
         <v>1.7525</v>
       </c>
       <c r="D51" s="1">
-        <v>1704.155</v>
+        <v>47716.34</v>
       </c>
       <c r="E51" s="2">
         <v>42036.0</v>
@@ -1392,7 +1386,7 @@
         <v>1.765</v>
       </c>
       <c r="D52" s="1">
-        <v>1864.075</v>
+        <v>52194.1</v>
       </c>
       <c r="E52" s="2">
         <v>42036.0</v>
@@ -1412,7 +1406,7 @@
         <v>1.715</v>
       </c>
       <c r="D53" s="1">
-        <v>7052.765</v>
+        <v>197477.42</v>
       </c>
       <c r="E53" s="2">
         <v>42036.0</v>
@@ -1432,7 +1426,7 @@
         <v>1.3</v>
       </c>
       <c r="D54" s="1">
-        <v>45898.885</v>
+        <v>1285168.78</v>
       </c>
       <c r="E54" s="2">
         <v>42036.0</v>
@@ -1452,7 +1446,7 @@
         <v>1.645</v>
       </c>
       <c r="D55" s="1">
-        <v>1330.8225</v>
+        <v>37263.03</v>
       </c>
       <c r="E55" s="2">
         <v>42036.0</v>
@@ -1472,7 +1466,7 @@
         <v>1.78</v>
       </c>
       <c r="D56" s="1">
-        <v>1766.08</v>
+        <v>49450.24</v>
       </c>
       <c r="E56" s="2">
         <v>42036.0</v>
@@ -1492,7 +1486,7 @@
         <v>1.43</v>
       </c>
       <c r="D57" s="1">
-        <v>7298.415</v>
+        <v>204355.62</v>
       </c>
       <c r="E57" s="2">
         <v>42036.0</v>
@@ -1512,7 +1506,7 @@
         <v>1.5025</v>
       </c>
       <c r="D58" s="1">
-        <v>3564.85</v>
+        <v>99815.8</v>
       </c>
       <c r="E58" s="2">
         <v>42036.0</v>
@@ -1532,7 +1526,7 @@
         <v>2.0</v>
       </c>
       <c r="D59" s="1">
-        <v>22231.85</v>
+        <v>622491.8</v>
       </c>
       <c r="E59" s="2">
         <v>42036.0</v>
@@ -1552,7 +1546,7 @@
         <v>1.8425</v>
       </c>
       <c r="D60" s="1">
-        <v>60990.5975</v>
+        <v>1707736.73</v>
       </c>
       <c r="E60" s="2">
         <v>42036.0</v>
@@ -1572,7 +1566,7 @@
         <v>1.865</v>
       </c>
       <c r="D61" s="1">
-        <v>6968.8075</v>
+        <v>195126.61</v>
       </c>
       <c r="E61" s="2">
         <v>42036.0</v>
@@ -1592,7 +1586,7 @@
         <v>1.058</v>
       </c>
       <c r="D62" s="1">
-        <v>3273549.272</v>
+        <v>1.01480027432E8</v>
       </c>
       <c r="E62" s="2">
         <v>42064.0</v>
@@ -1612,7 +1606,7 @@
         <v>1.128</v>
       </c>
       <c r="D63" s="1">
-        <v>206076.672</v>
+        <v>6388376.832</v>
       </c>
       <c r="E63" s="2">
         <v>42064.0</v>
@@ -1632,7 +1626,7 @@
         <v>1.256</v>
       </c>
       <c r="D64" s="1">
-        <v>257074.158</v>
+        <v>7969298.898</v>
       </c>
       <c r="E64" s="2">
         <v>42064.0</v>
@@ -1652,7 +1646,7 @@
         <v>0.802</v>
       </c>
       <c r="D65" s="1">
-        <v>1070689.224</v>
+        <v>3.3191365944E7</v>
       </c>
       <c r="E65" s="2">
         <v>42064.0</v>
@@ -1672,7 +1666,7 @@
         <v>1.122</v>
       </c>
       <c r="D66" s="1">
-        <v>158465.768</v>
+        <v>4912438.808</v>
       </c>
       <c r="E66" s="2">
         <v>42064.0</v>
@@ -1692,7 +1686,7 @@
         <v>1.136</v>
       </c>
       <c r="D67" s="1">
-        <v>136898.134</v>
+        <v>4243842.154</v>
       </c>
       <c r="E67" s="2">
         <v>42064.0</v>
@@ -1712,7 +1706,7 @@
         <v>0.974</v>
       </c>
       <c r="D68" s="1">
-        <v>302202.118</v>
+        <v>9368265.658</v>
       </c>
       <c r="E68" s="2">
         <v>42064.0</v>
@@ -1732,7 +1726,7 @@
         <v>0.912</v>
       </c>
       <c r="D69" s="1">
-        <v>2723141.526</v>
+        <v>8.4417387306E7</v>
       </c>
       <c r="E69" s="2">
         <v>42064.0</v>
@@ -1752,7 +1746,7 @@
         <v>1.08</v>
       </c>
       <c r="D70" s="1">
-        <v>77425.858</v>
+        <v>2400201.598</v>
       </c>
       <c r="E70" s="2">
         <v>42064.0</v>
@@ -1772,7 +1766,7 @@
         <v>1.172</v>
       </c>
       <c r="D71" s="1">
-        <v>477608.418</v>
+        <v>1.4805860958E7</v>
       </c>
       <c r="E71" s="2">
         <v>42064.0</v>
@@ -1792,7 +1786,7 @@
         <v>1.046</v>
       </c>
       <c r="D72" s="1">
-        <v>154999.644</v>
+        <v>4804988.964</v>
       </c>
       <c r="E72" s="2">
         <v>42064.0</v>
@@ -1812,7 +1806,7 @@
         <v>1.02</v>
       </c>
       <c r="D73" s="1">
-        <v>245280.952</v>
+        <v>7603709.512</v>
       </c>
       <c r="E73" s="2">
         <v>42064.0</v>
@@ -1832,7 +1826,7 @@
         <v>1.336</v>
       </c>
       <c r="D74" s="1">
-        <v>1188349.892</v>
+        <v>3.6838846652E7</v>
       </c>
       <c r="E74" s="2">
         <v>42064.0</v>
@@ -1852,7 +1846,7 @@
         <v>1.248</v>
       </c>
       <c r="D75" s="1">
-        <v>3436943.066</v>
+        <v>1.06545235046E8</v>
       </c>
       <c r="E75" s="2">
         <v>42064.0</v>
@@ -1872,7 +1866,7 @@
         <v>1.11</v>
       </c>
       <c r="D76" s="1">
-        <v>328057.754</v>
+        <v>1.0169790374E7</v>
       </c>
       <c r="E76" s="2">
         <v>42064.0</v>
@@ -1892,7 +1886,7 @@
         <v>1.618</v>
       </c>
       <c r="D77" s="1">
-        <v>64409.738</v>
+        <v>1996701.878</v>
       </c>
       <c r="E77" s="2">
         <v>42064.0</v>
@@ -1912,7 +1906,7 @@
         <v>1.788</v>
       </c>
       <c r="D78" s="1">
-        <v>3287.536</v>
+        <v>101913.616</v>
       </c>
       <c r="E78" s="2">
         <v>42064.0</v>
@@ -1932,7 +1926,7 @@
         <v>2.212</v>
       </c>
       <c r="D79" s="1">
-        <v>2826.546</v>
+        <v>87622.926</v>
       </c>
       <c r="E79" s="2">
         <v>42064.0</v>
@@ -1952,7 +1946,7 @@
         <v>1.252</v>
       </c>
       <c r="D80" s="1">
-        <v>10910.094</v>
+        <v>338212.914</v>
       </c>
       <c r="E80" s="2">
         <v>42064.0</v>
@@ -1972,7 +1966,7 @@
         <v>1.804</v>
       </c>
       <c r="D81" s="1">
-        <v>1455.458</v>
+        <v>45119.198</v>
       </c>
       <c r="E81" s="2">
         <v>42064.0</v>
@@ -1992,7 +1986,7 @@
         <v>1.792</v>
       </c>
       <c r="D82" s="1">
-        <v>2118.164</v>
+        <v>65663.084</v>
       </c>
       <c r="E82" s="2">
         <v>42064.0</v>
@@ -2012,7 +2006,7 @@
         <v>1.634</v>
       </c>
       <c r="D83" s="1">
-        <v>7426.004</v>
+        <v>230206.124</v>
       </c>
       <c r="E83" s="2">
         <v>42064.0</v>
@@ -2032,7 +2026,7 @@
         <v>1.316</v>
       </c>
       <c r="D84" s="1">
-        <v>42348.53</v>
+        <v>1312804.43</v>
       </c>
       <c r="E84" s="2">
         <v>42064.0</v>
@@ -2052,7 +2046,7 @@
         <v>1.682</v>
       </c>
       <c r="D85" s="1">
-        <v>1393.456</v>
+        <v>43197.136</v>
       </c>
       <c r="E85" s="2">
         <v>42064.0</v>
@@ -2072,7 +2066,7 @@
         <v>1.764</v>
       </c>
       <c r="D86" s="1">
-        <v>2340.176</v>
+        <v>72545.456</v>
       </c>
       <c r="E86" s="2">
         <v>42064.0</v>
@@ -2092,7 +2086,7 @@
         <v>1.73</v>
       </c>
       <c r="D87" s="1">
-        <v>3993.808</v>
+        <v>123808.048</v>
       </c>
       <c r="E87" s="2">
         <v>42064.0</v>
@@ -2112,7 +2106,7 @@
         <v>1.574</v>
       </c>
       <c r="D88" s="1">
-        <v>2581.378</v>
+        <v>80022.718</v>
       </c>
       <c r="E88" s="2">
         <v>42064.0</v>
@@ -2132,7 +2126,7 @@
         <v>1.962</v>
       </c>
       <c r="D89" s="1">
-        <v>17853.652</v>
+        <v>553463.212</v>
       </c>
       <c r="E89" s="2">
         <v>42064.0</v>
@@ -2152,7 +2146,7 @@
         <v>1.868</v>
       </c>
       <c r="D90" s="1">
-        <v>50218.56</v>
+        <v>1556775.36</v>
       </c>
       <c r="E90" s="2">
         <v>42064.0</v>
@@ -2172,7 +2166,7 @@
         <v>1.874</v>
       </c>
       <c r="D91" s="1">
-        <v>6762.936</v>
+        <v>209651.016</v>
       </c>
       <c r="E91" s="2">
         <v>42064.0</v>
@@ -2192,7 +2186,7 @@
         <v>1.1225</v>
       </c>
       <c r="D92" s="1">
-        <v>3231635.285</v>
+        <v>9.694905855E7</v>
       </c>
       <c r="E92" s="2">
         <v>42095.0</v>
@@ -2212,7 +2206,7 @@
         <v>1.1925</v>
       </c>
       <c r="D93" s="1">
-        <v>222418.12</v>
+        <v>6672543.6</v>
       </c>
       <c r="E93" s="2">
         <v>42095.0</v>
@@ -2232,7 +2226,7 @@
         <v>1.3225</v>
       </c>
       <c r="D94" s="1">
-        <v>261606.9375</v>
+        <v>7848208.125</v>
       </c>
       <c r="E94" s="2">
         <v>42095.0</v>
@@ -2252,7 +2246,7 @@
         <v>0.8075</v>
       </c>
       <c r="D95" s="1">
-        <v>1090246.3075</v>
+        <v>3.2707389225E7</v>
       </c>
       <c r="E95" s="2">
         <v>42095.0</v>
@@ -2272,7 +2266,7 @@
         <v>1.16</v>
       </c>
       <c r="D96" s="1">
-        <v>158821.26</v>
+        <v>4764637.8</v>
       </c>
       <c r="E96" s="2">
         <v>42095.0</v>
@@ -2292,7 +2286,7 @@
         <v>1.1175</v>
       </c>
       <c r="D97" s="1">
-        <v>145112.4675</v>
+        <v>4353374.025</v>
       </c>
       <c r="E97" s="2">
         <v>42095.0</v>
@@ -2312,7 +2306,7 @@
         <v>0.8175</v>
       </c>
       <c r="D98" s="1">
-        <v>350353.405</v>
+        <v>1.051060215E7</v>
       </c>
       <c r="E98" s="2">
         <v>42095.0</v>
@@ -2332,7 +2326,7 @@
         <v>0.9725</v>
       </c>
       <c r="D99" s="1">
-        <v>2664918.5025</v>
+        <v>7.9947555075E7</v>
       </c>
       <c r="E99" s="2">
         <v>42095.0</v>
@@ -2352,7 +2346,7 @@
         <v>1.0675</v>
       </c>
       <c r="D100" s="1">
-        <v>81390.9925</v>
+        <v>2441729.775</v>
       </c>
       <c r="E100" s="2">
         <v>42095.0</v>
@@ -2372,7 +2366,7 @@
         <v>1.1475</v>
       </c>
       <c r="D101" s="1">
-        <v>528337.8125</v>
+        <v>1.5850134375E7</v>
       </c>
       <c r="E101" s="2">
         <v>42095.0</v>
@@ -2392,7 +2386,7 @@
         <v>1.0625</v>
       </c>
       <c r="D102" s="1">
-        <v>155192.6225</v>
+        <v>4655778.675</v>
       </c>
       <c r="E102" s="2">
         <v>42095.0</v>
@@ -2412,7 +2406,7 @@
         <v>0.9625</v>
       </c>
       <c r="D103" s="1">
-        <v>250689.505</v>
+        <v>7520685.15</v>
       </c>
       <c r="E103" s="2">
         <v>42095.0</v>
@@ -2432,7 +2426,7 @@
         <v>1.425</v>
       </c>
       <c r="D104" s="1">
-        <v>1239209.1275</v>
+        <v>3.7176273825E7</v>
       </c>
       <c r="E104" s="2">
         <v>42095.0</v>
@@ -2452,7 +2446,7 @@
         <v>1.335</v>
       </c>
       <c r="D105" s="1">
-        <v>3525872.16</v>
+        <v>1.057761648E8</v>
       </c>
       <c r="E105" s="2">
         <v>42095.0</v>
@@ -2472,7 +2466,7 @@
         <v>1.18</v>
       </c>
       <c r="D106" s="1">
-        <v>318458.8275</v>
+        <v>9553764.825</v>
       </c>
       <c r="E106" s="2">
         <v>42095.0</v>
@@ -2492,7 +2486,7 @@
         <v>1.5125</v>
       </c>
       <c r="D107" s="1">
-        <v>102380.16</v>
+        <v>3071404.8</v>
       </c>
       <c r="E107" s="2">
         <v>42095.0</v>
@@ -2512,7 +2506,7 @@
         <v>1.8075</v>
       </c>
       <c r="D108" s="1">
-        <v>3421.0625</v>
+        <v>102631.875</v>
       </c>
       <c r="E108" s="2">
         <v>42095.0</v>
@@ -2532,7 +2526,7 @@
         <v>2.2125</v>
       </c>
       <c r="D109" s="1">
-        <v>3178.825</v>
+        <v>95364.75</v>
       </c>
       <c r="E109" s="2">
         <v>42095.0</v>
@@ -2552,7 +2546,7 @@
         <v>1.2575</v>
       </c>
       <c r="D110" s="1">
-        <v>12495.0725</v>
+        <v>374852.175</v>
       </c>
       <c r="E110" s="2">
         <v>42095.0</v>
@@ -2572,7 +2566,7 @@
         <v>1.68</v>
       </c>
       <c r="D111" s="1">
-        <v>1938.015</v>
+        <v>58140.45</v>
       </c>
       <c r="E111" s="2">
         <v>42095.0</v>
@@ -2592,7 +2586,7 @@
         <v>1.85</v>
       </c>
       <c r="D112" s="1">
-        <v>1964.175</v>
+        <v>58925.25</v>
       </c>
       <c r="E112" s="2">
         <v>42095.0</v>
@@ -2612,7 +2606,7 @@
         <v>1.605</v>
       </c>
       <c r="D113" s="1">
-        <v>10303.2175</v>
+        <v>309096.525</v>
       </c>
       <c r="E113" s="2">
         <v>42095.0</v>
@@ -2632,7 +2626,7 @@
         <v>1.405</v>
       </c>
       <c r="D114" s="1">
-        <v>44292.9325</v>
+        <v>1328787.975</v>
       </c>
       <c r="E114" s="2">
         <v>42095.0</v>
@@ -2652,7 +2646,7 @@
         <v>1.5125</v>
       </c>
       <c r="D115" s="1">
-        <v>1565.965</v>
+        <v>46978.95</v>
       </c>
       <c r="E115" s="2">
         <v>42095.0</v>
@@ -2672,7 +2666,7 @@
         <v>1.6325</v>
       </c>
       <c r="D116" s="1">
-        <v>3272.6575</v>
+        <v>98179.725</v>
       </c>
       <c r="E116" s="2">
         <v>42095.0</v>
@@ -2692,7 +2686,7 @@
         <v>1.5725</v>
       </c>
       <c r="D117" s="1">
-        <v>6461.875</v>
+        <v>193856.25</v>
       </c>
       <c r="E117" s="2">
         <v>42095.0</v>
@@ -2712,7 +2706,7 @@
         <v>1.56</v>
       </c>
       <c r="D118" s="1">
-        <v>3137.3475</v>
+        <v>94120.425</v>
       </c>
       <c r="E118" s="2">
         <v>42095.0</v>
@@ -2732,7 +2726,7 @@
         <v>2.0625</v>
       </c>
       <c r="D119" s="1">
-        <v>20254.6075</v>
+        <v>607638.225</v>
       </c>
       <c r="E119" s="2">
         <v>42095.0</v>
@@ -2752,7 +2746,7 @@
         <v>1.905</v>
       </c>
       <c r="D120" s="1">
-        <v>58974.1275</v>
+        <v>1769223.825</v>
       </c>
       <c r="E120" s="2">
         <v>42095.0</v>
@@ -2772,7 +2766,7 @@
         <v>1.8775</v>
       </c>
       <c r="D121" s="1">
-        <v>7647.9775</v>
+        <v>229439.325</v>
       </c>
       <c r="E121" s="2">
         <v>42095.0</v>
@@ -2792,7 +2786,7 @@
         <v>1.128</v>
       </c>
       <c r="D122" s="1">
-        <v>3576272.904</v>
+        <v>1.10864460024E8</v>
       </c>
       <c r="E122" s="2">
         <v>42125.0</v>
@@ -2812,7 +2806,7 @@
         <v>1.196</v>
       </c>
       <c r="D123" s="1">
-        <v>267612.236</v>
+        <v>8295979.316</v>
       </c>
       <c r="E123" s="2">
         <v>42125.0</v>
@@ -2832,7 +2826,7 @@
         <v>1.274</v>
       </c>
       <c r="D124" s="1">
-        <v>338739.952</v>
+        <v>1.0500938512E7</v>
       </c>
       <c r="E124" s="2">
         <v>42125.0</v>
@@ -2852,7 +2846,7 @@
         <v>0.774</v>
       </c>
       <c r="D125" s="1">
-        <v>1175250.596</v>
+        <v>3.6432768476E7</v>
       </c>
       <c r="E125" s="2">
         <v>42125.0</v>
@@ -2872,7 +2866,7 @@
         <v>1.222</v>
       </c>
       <c r="D126" s="1">
-        <v>170022.964</v>
+        <v>5270711.884</v>
       </c>
       <c r="E126" s="2">
         <v>42125.0</v>
@@ -2892,7 +2886,7 @@
         <v>1.132</v>
       </c>
       <c r="D127" s="1">
-        <v>164913.224</v>
+        <v>5112309.944</v>
       </c>
       <c r="E127" s="2">
         <v>42125.0</v>
@@ -2912,7 +2906,7 @@
         <v>0.976</v>
       </c>
       <c r="D128" s="1">
-        <v>318113.864</v>
+        <v>9861529.784</v>
       </c>
       <c r="E128" s="2">
         <v>42125.0</v>
@@ -2932,7 +2926,7 @@
         <v>0.872</v>
       </c>
       <c r="D129" s="1">
-        <v>3235549.4</v>
+        <v>1.003020314E8</v>
       </c>
       <c r="E129" s="2">
         <v>42125.0</v>
@@ -2952,7 +2946,7 @@
         <v>1.076</v>
       </c>
       <c r="D130" s="1">
-        <v>85289.414</v>
+        <v>2643971.834</v>
       </c>
       <c r="E130" s="2">
         <v>42125.0</v>
@@ -2972,7 +2966,7 @@
         <v>1.156</v>
       </c>
       <c r="D131" s="1">
-        <v>596007.828</v>
+        <v>1.8476242668E7</v>
       </c>
       <c r="E131" s="2">
         <v>42125.0</v>
@@ -2992,7 +2986,7 @@
         <v>1.028</v>
       </c>
       <c r="D132" s="1">
-        <v>179828.98</v>
+        <v>5574698.38</v>
       </c>
       <c r="E132" s="2">
         <v>42125.0</v>
@@ -3012,7 +3006,7 @@
         <v>1.002</v>
       </c>
       <c r="D133" s="1">
-        <v>266576.3</v>
+        <v>8263865.3</v>
       </c>
       <c r="E133" s="2">
         <v>42125.0</v>
@@ -3032,7 +3026,7 @@
         <v>1.354</v>
       </c>
       <c r="D134" s="1">
-        <v>1612298.274</v>
+        <v>4.9981246494E7</v>
       </c>
       <c r="E134" s="2">
         <v>42125.0</v>
@@ -3052,7 +3046,7 @@
         <v>1.276</v>
       </c>
       <c r="D135" s="1">
-        <v>4636267.73</v>
+        <v>1.4372429963E8</v>
       </c>
       <c r="E135" s="2">
         <v>42125.0</v>
@@ -3072,7 +3066,7 @@
         <v>1.12</v>
       </c>
       <c r="D136" s="1">
-        <v>458756.078</v>
+        <v>1.4221438418E7</v>
       </c>
       <c r="E136" s="2">
         <v>42125.0</v>
@@ -3092,9 +3086,9 @@
         <v>1.42</v>
       </c>
       <c r="D137" s="1">
-        <v>111413.84</v>
-      </c>
-      <c r="E137" s="3">
+        <v>3453829.04</v>
+      </c>
+      <c r="E137" s="2">
         <v>42125.0</v>
       </c>
       <c r="F137" s="1" t="s">
@@ -3112,9 +3106,9 @@
         <v>1.834</v>
       </c>
       <c r="D138" s="1">
-        <v>3976.616</v>
-      </c>
-      <c r="E138" s="3">
+        <v>123275.096</v>
+      </c>
+      <c r="E138" s="2">
         <v>42125.0</v>
       </c>
       <c r="F138" s="1" t="s">
@@ -3132,9 +3126,9 @@
         <v>2.152</v>
       </c>
       <c r="D139" s="1">
-        <v>4217.374</v>
-      </c>
-      <c r="E139" s="3">
+        <v>130738.594</v>
+      </c>
+      <c r="E139" s="2">
         <v>42125.0</v>
       </c>
       <c r="F139" s="1" t="s">
@@ -3152,9 +3146,9 @@
         <v>1.256</v>
       </c>
       <c r="D140" s="1">
-        <v>10506.796</v>
-      </c>
-      <c r="E140" s="3">
+        <v>325710.676</v>
+      </c>
+      <c r="E140" s="2">
         <v>42125.0</v>
       </c>
       <c r="F140" s="1" t="s">
@@ -3172,9 +3166,9 @@
         <v>1.356</v>
       </c>
       <c r="D141" s="1">
-        <v>2691.842</v>
-      </c>
-      <c r="E141" s="3">
+        <v>83447.102</v>
+      </c>
+      <c r="E141" s="2">
         <v>42125.0</v>
       </c>
       <c r="F141" s="1" t="s">
@@ -3192,9 +3186,9 @@
         <v>1.808</v>
       </c>
       <c r="D142" s="1">
-        <v>2267.286</v>
-      </c>
-      <c r="E142" s="3">
+        <v>70285.866</v>
+      </c>
+      <c r="E142" s="2">
         <v>42125.0</v>
       </c>
       <c r="F142" s="1" t="s">
@@ -3212,9 +3206,9 @@
         <v>1.356</v>
       </c>
       <c r="D143" s="1">
-        <v>11383.484</v>
-      </c>
-      <c r="E143" s="3">
+        <v>352888.004</v>
+      </c>
+      <c r="E143" s="2">
         <v>42125.0</v>
       </c>
       <c r="F143" s="1" t="s">
@@ -3232,9 +3226,9 @@
         <v>1.396</v>
       </c>
       <c r="D144" s="1">
-        <v>44566.272</v>
-      </c>
-      <c r="E144" s="3">
+        <v>1381554.432</v>
+      </c>
+      <c r="E144" s="2">
         <v>42125.0</v>
       </c>
       <c r="F144" s="1" t="s">
@@ -3252,9 +3246,9 @@
         <v>1.342</v>
       </c>
       <c r="D145" s="1">
-        <v>2383.09</v>
-      </c>
-      <c r="E145" s="3">
+        <v>73875.79</v>
+      </c>
+      <c r="E145" s="2">
         <v>42125.0</v>
       </c>
       <c r="F145" s="1" t="s">
@@ -3272,9 +3266,9 @@
         <v>1.68</v>
       </c>
       <c r="D146" s="1">
-        <v>2697.258</v>
-      </c>
-      <c r="E146" s="3">
+        <v>83614.998</v>
+      </c>
+      <c r="E146" s="2">
         <v>42125.0</v>
       </c>
       <c r="F146" s="1" t="s">
@@ -3292,9 +3286,9 @@
         <v>1.43</v>
       </c>
       <c r="D147" s="1">
-        <v>6385.096</v>
-      </c>
-      <c r="E147" s="3">
+        <v>197937.976</v>
+      </c>
+      <c r="E147" s="2">
         <v>42125.0</v>
       </c>
       <c r="F147" s="1" t="s">
@@ -3312,9 +3306,9 @@
         <v>1.568</v>
       </c>
       <c r="D148" s="1">
-        <v>1808.592</v>
-      </c>
-      <c r="E148" s="3">
+        <v>56066.352</v>
+      </c>
+      <c r="E148" s="2">
         <v>42125.0</v>
       </c>
       <c r="F148" s="1" t="s">
@@ -3332,9 +3326,9 @@
         <v>2.046</v>
       </c>
       <c r="D149" s="1">
-        <v>19995.894</v>
-      </c>
-      <c r="E149" s="3">
+        <v>619872.714</v>
+      </c>
+      <c r="E149" s="2">
         <v>42125.0</v>
       </c>
       <c r="F149" s="1" t="s">
@@ -3352,9 +3346,9 @@
         <v>1.914</v>
       </c>
       <c r="D150" s="1">
-        <v>66525.212</v>
-      </c>
-      <c r="E150" s="3">
+        <v>2062281.572</v>
+      </c>
+      <c r="E150" s="2">
         <v>42125.0</v>
       </c>
       <c r="F150" s="1" t="s">
@@ -3372,9 +3366,9 @@
         <v>1.9</v>
       </c>
       <c r="D151" s="1">
-        <v>8034.342</v>
-      </c>
-      <c r="E151" s="3">
+        <v>249064.602</v>
+      </c>
+      <c r="E151" s="2">
         <v>42125.0</v>
       </c>
       <c r="F151" s="1" t="s">
@@ -3392,7 +3386,7 @@
         <v>1.1</v>
       </c>
       <c r="D152" s="1">
-        <v>3542517.7775</v>
+        <v>1.06275533325E8</v>
       </c>
       <c r="E152" s="2">
         <v>42156.0</v>
@@ -3412,7 +3406,7 @@
         <v>1.1825</v>
       </c>
       <c r="D153" s="1">
-        <v>260546.61</v>
+        <v>7816398.3</v>
       </c>
       <c r="E153" s="2">
         <v>42156.0</v>
@@ -3432,7 +3426,7 @@
         <v>1.24</v>
       </c>
       <c r="D154" s="1">
-        <v>334441.0925</v>
+        <v>1.0033232775E7</v>
       </c>
       <c r="E154" s="2">
         <v>42156.0</v>
@@ -3452,7 +3446,7 @@
         <v>0.705</v>
       </c>
       <c r="D155" s="1">
-        <v>1259405.825</v>
+        <v>3.778217475E7</v>
       </c>
       <c r="E155" s="2">
         <v>42156.0</v>
@@ -3472,7 +3466,7 @@
         <v>1.1025</v>
       </c>
       <c r="D156" s="1">
-        <v>183185.5525</v>
+        <v>5495566.575</v>
       </c>
       <c r="E156" s="2">
         <v>42156.0</v>
@@ -3492,7 +3486,7 @@
         <v>1.0725</v>
       </c>
       <c r="D157" s="1">
-        <v>161943.6675</v>
+        <v>4858310.025</v>
       </c>
       <c r="E157" s="2">
         <v>42156.0</v>
@@ -3512,7 +3506,7 @@
         <v>0.9525</v>
       </c>
       <c r="D158" s="1">
-        <v>339335.16</v>
+        <v>1.01800548E7</v>
       </c>
       <c r="E158" s="2">
         <v>42156.0</v>
@@ -3532,7 +3526,7 @@
         <v>0.87</v>
       </c>
       <c r="D159" s="1">
-        <v>3228039.3975</v>
+        <v>9.6841181925E7</v>
       </c>
       <c r="E159" s="2">
         <v>42156.0</v>
@@ -3552,7 +3546,7 @@
         <v>1.1</v>
       </c>
       <c r="D160" s="1">
-        <v>82183.2575</v>
+        <v>2465497.725</v>
       </c>
       <c r="E160" s="2">
         <v>42156.0</v>
@@ -3572,7 +3566,7 @@
         <v>1.105</v>
       </c>
       <c r="D161" s="1">
-        <v>558788.5625</v>
+        <v>1.6763656875E7</v>
       </c>
       <c r="E161" s="2">
         <v>42156.0</v>
@@ -3592,7 +3586,7 @@
         <v>1.0025</v>
       </c>
       <c r="D162" s="1">
-        <v>177629.2825</v>
+        <v>5328878.475</v>
       </c>
       <c r="E162" s="2">
         <v>42156.0</v>
@@ -3612,7 +3606,7 @@
         <v>0.9925</v>
       </c>
       <c r="D163" s="1">
-        <v>276511.035</v>
+        <v>8295331.05</v>
       </c>
       <c r="E163" s="2">
         <v>42156.0</v>
@@ -3632,7 +3626,7 @@
         <v>1.32</v>
       </c>
       <c r="D164" s="1">
-        <v>1511502.66</v>
+        <v>4.53450798E7</v>
       </c>
       <c r="E164" s="2">
         <v>42156.0</v>
@@ -3652,7 +3646,7 @@
         <v>1.26</v>
       </c>
       <c r="D165" s="1">
-        <v>4473270.8575</v>
+        <v>1.34198125725E8</v>
       </c>
       <c r="E165" s="2">
         <v>42156.0</v>
@@ -3672,7 +3666,7 @@
         <v>1.1325</v>
       </c>
       <c r="D166" s="1">
-        <v>460907.185</v>
+        <v>1.382721555E7</v>
       </c>
       <c r="E166" s="2">
         <v>42156.0</v>
@@ -3692,7 +3686,7 @@
         <v>1.585</v>
       </c>
       <c r="D167" s="1">
-        <v>76775.265</v>
+        <v>2303257.95</v>
       </c>
       <c r="E167" s="2">
         <v>42156.0</v>
@@ -3712,7 +3706,7 @@
         <v>1.855</v>
       </c>
       <c r="D168" s="1">
-        <v>3360.58</v>
+        <v>100817.4</v>
       </c>
       <c r="E168" s="2">
         <v>42156.0</v>
@@ -3732,7 +3726,7 @@
         <v>2.325</v>
       </c>
       <c r="D169" s="1">
-        <v>3399.095</v>
+        <v>101972.85</v>
       </c>
       <c r="E169" s="2">
         <v>42156.0</v>
@@ -3752,7 +3746,7 @@
         <v>1.2075</v>
       </c>
       <c r="D170" s="1">
-        <v>10799.9725</v>
+        <v>323999.175</v>
       </c>
       <c r="E170" s="2">
         <v>42156.0</v>
@@ -3772,7 +3766,7 @@
         <v>1.6</v>
       </c>
       <c r="D171" s="1">
-        <v>1817.555</v>
+        <v>54526.65</v>
       </c>
       <c r="E171" s="2">
         <v>42156.0</v>
@@ -3792,7 +3786,7 @@
         <v>1.8475</v>
       </c>
       <c r="D172" s="1">
-        <v>2521.965</v>
+        <v>75658.95</v>
       </c>
       <c r="E172" s="2">
         <v>42156.0</v>
@@ -3812,7 +3806,7 @@
         <v>1.48</v>
       </c>
       <c r="D173" s="1">
-        <v>10869.9075</v>
+        <v>326097.225</v>
       </c>
       <c r="E173" s="2">
         <v>42156.0</v>
@@ -3832,7 +3826,7 @@
         <v>1.4475</v>
       </c>
       <c r="D174" s="1">
-        <v>45044.4625</v>
+        <v>1351333.875</v>
       </c>
       <c r="E174" s="2">
         <v>42156.0</v>
@@ -3852,7 +3846,7 @@
         <v>1.4425</v>
       </c>
       <c r="D175" s="1">
-        <v>2120.455</v>
+        <v>63613.65</v>
       </c>
       <c r="E175" s="2">
         <v>42156.0</v>
@@ -3872,7 +3866,7 @@
         <v>1.835</v>
       </c>
       <c r="D176" s="1">
-        <v>1788.6775</v>
+        <v>53660.325</v>
       </c>
       <c r="E176" s="2">
         <v>42156.0</v>
@@ -3892,7 +3886,7 @@
         <v>1.57</v>
       </c>
       <c r="D177" s="1">
-        <v>5715.1975</v>
+        <v>171455.925</v>
       </c>
       <c r="E177" s="2">
         <v>42156.0</v>
@@ -3912,7 +3906,7 @@
         <v>1.605</v>
       </c>
       <c r="D178" s="1">
-        <v>2322.885</v>
+        <v>69686.55</v>
       </c>
       <c r="E178" s="2">
         <v>42156.0</v>
@@ -3932,7 +3926,7 @@
         <v>2.145</v>
       </c>
       <c r="D179" s="1">
-        <v>17786.345</v>
+        <v>533590.35</v>
       </c>
       <c r="E179" s="2">
         <v>42156.0</v>
@@ -3952,7 +3946,7 @@
         <v>2.0</v>
       </c>
       <c r="D180" s="1">
-        <v>57127.1575</v>
+        <v>1713814.725</v>
       </c>
       <c r="E180" s="2">
         <v>42156.0</v>
@@ -3972,7 +3966,7 @@
         <v>1.935</v>
       </c>
       <c r="D181" s="1">
-        <v>8317.245</v>
+        <v>249517.35</v>
       </c>
       <c r="E181" s="2">
         <v>42156.0</v>
@@ -3992,7 +3986,7 @@
         <v>1.1225</v>
       </c>
       <c r="D182" s="1">
-        <v>3355951.045</v>
+        <v>1.04034482395E8</v>
       </c>
       <c r="E182" s="2">
         <v>42186.0</v>
@@ -4012,7 +4006,7 @@
         <v>1.18</v>
       </c>
       <c r="D183" s="1">
-        <v>241090.495</v>
+        <v>7473805.345</v>
       </c>
       <c r="E183" s="2">
         <v>42186.0</v>
@@ -4032,7 +4026,7 @@
         <v>1.2325</v>
       </c>
       <c r="D184" s="1">
-        <v>313283.775</v>
+        <v>9711797.025</v>
       </c>
       <c r="E184" s="2">
         <v>42186.0</v>
@@ -4052,7 +4046,7 @@
         <v>0.7875</v>
       </c>
       <c r="D185" s="1">
-        <v>1088397.99</v>
+        <v>3.374033769E7</v>
       </c>
       <c r="E185" s="2">
         <v>42186.0</v>
@@ -4072,7 +4066,7 @@
         <v>1.0975</v>
       </c>
       <c r="D186" s="1">
-        <v>166197.2325</v>
+        <v>5152114.2075</v>
       </c>
       <c r="E186" s="2">
         <v>42186.0</v>
@@ -4092,7 +4086,7 @@
         <v>1.105</v>
       </c>
       <c r="D187" s="1">
-        <v>152415.855</v>
+        <v>4724891.505</v>
       </c>
       <c r="E187" s="2">
         <v>42186.0</v>
@@ -4112,7 +4106,7 @@
         <v>1.04</v>
       </c>
       <c r="D188" s="1">
-        <v>288118.14</v>
+        <v>8931662.34</v>
       </c>
       <c r="E188" s="2">
         <v>42186.0</v>
@@ -4132,7 +4126,7 @@
         <v>0.99</v>
       </c>
       <c r="D189" s="1">
-        <v>2899117.265</v>
+        <v>8.9872635215E7</v>
       </c>
       <c r="E189" s="2">
         <v>42186.0</v>
@@ -4152,7 +4146,7 @@
         <v>1.06</v>
       </c>
       <c r="D190" s="1">
-        <v>82872.825</v>
+        <v>2569057.575</v>
       </c>
       <c r="E190" s="2">
         <v>42186.0</v>
@@ -4172,7 +4166,7 @@
         <v>1.105</v>
       </c>
       <c r="D191" s="1">
-        <v>531913.685</v>
+        <v>1.6489324235E7</v>
       </c>
       <c r="E191" s="2">
         <v>42186.0</v>
@@ -4192,7 +4186,7 @@
         <v>1.0275</v>
       </c>
       <c r="D192" s="1">
-        <v>172577.865</v>
+        <v>5349913.815</v>
       </c>
       <c r="E192" s="2">
         <v>42186.0</v>
@@ -4212,7 +4206,7 @@
         <v>1.0175</v>
       </c>
       <c r="D193" s="1">
-        <v>263727.3725</v>
+        <v>8175548.5475</v>
       </c>
       <c r="E193" s="2">
         <v>42186.0</v>
@@ -4232,7 +4226,7 @@
         <v>1.275</v>
       </c>
       <c r="D194" s="1">
-        <v>1367189.575</v>
+        <v>4.2382876825E7</v>
       </c>
       <c r="E194" s="2">
         <v>42186.0</v>
@@ -4252,7 +4246,7 @@
         <v>1.2475</v>
       </c>
       <c r="D195" s="1">
-        <v>4309037.6325</v>
+        <v>1.335801666075E8</v>
       </c>
       <c r="E195" s="2">
         <v>42186.0</v>
@@ -4272,7 +4266,7 @@
         <v>1.1325</v>
       </c>
       <c r="D196" s="1">
-        <v>510775.48</v>
+        <v>1.583403988E7</v>
       </c>
       <c r="E196" s="2">
         <v>42186.0</v>
@@ -4292,7 +4286,7 @@
         <v>1.48</v>
       </c>
       <c r="D197" s="1">
-        <v>85826.625</v>
+        <v>2660625.375</v>
       </c>
       <c r="E197" s="2">
         <v>42186.0</v>
@@ -4312,7 +4306,7 @@
         <v>1.9775</v>
       </c>
       <c r="D198" s="1">
-        <v>1914.38</v>
+        <v>59345.78</v>
       </c>
       <c r="E198" s="2">
         <v>42186.0</v>
@@ -4332,7 +4326,7 @@
         <v>2.405</v>
       </c>
       <c r="D199" s="1">
-        <v>3176.5475</v>
+        <v>98472.9725</v>
       </c>
       <c r="E199" s="2">
         <v>42186.0</v>
@@ -4352,7 +4346,7 @@
         <v>1.185</v>
       </c>
       <c r="D200" s="1">
-        <v>12001.315</v>
+        <v>372040.765</v>
       </c>
       <c r="E200" s="2">
         <v>42186.0</v>
@@ -4372,7 +4366,7 @@
         <v>1.1</v>
       </c>
       <c r="D201" s="1">
-        <v>3081.685</v>
+        <v>95532.235</v>
       </c>
       <c r="E201" s="2">
         <v>42186.0</v>
@@ -4392,7 +4386,7 @@
         <v>1.81</v>
       </c>
       <c r="D202" s="1">
-        <v>2995.0875</v>
+        <v>92847.7125</v>
       </c>
       <c r="E202" s="2">
         <v>42186.0</v>
@@ -4412,7 +4406,7 @@
         <v>1.865</v>
       </c>
       <c r="D203" s="1">
-        <v>6831.585</v>
+        <v>211779.135</v>
       </c>
       <c r="E203" s="2">
         <v>42186.0</v>
@@ -4432,7 +4426,7 @@
         <v>1.535</v>
       </c>
       <c r="D204" s="1">
-        <v>45385.4275</v>
+        <v>1406948.2525</v>
       </c>
       <c r="E204" s="2">
         <v>42186.0</v>
@@ -4452,7 +4446,7 @@
         <v>1.295</v>
       </c>
       <c r="D205" s="1">
-        <v>2520.8</v>
+        <v>78144.8</v>
       </c>
       <c r="E205" s="2">
         <v>42186.0</v>
@@ -4472,7 +4466,7 @@
         <v>1.5925</v>
       </c>
       <c r="D206" s="1">
-        <v>1220.5325</v>
+        <v>37836.5075</v>
       </c>
       <c r="E206" s="2">
         <v>42186.0</v>
@@ -4492,7 +4486,7 @@
         <v>1.2225</v>
       </c>
       <c r="D207" s="1">
-        <v>7952.1475</v>
+        <v>246516.5725</v>
       </c>
       <c r="E207" s="2">
         <v>42186.0</v>
@@ -4512,7 +4506,7 @@
         <v>1.5425</v>
       </c>
       <c r="D208" s="1">
-        <v>2040.5</v>
+        <v>63255.5</v>
       </c>
       <c r="E208" s="2">
         <v>42186.0</v>
@@ -4532,7 +4526,7 @@
         <v>2.0925</v>
       </c>
       <c r="D209" s="1">
-        <v>11712.1875</v>
+        <v>363077.8125</v>
       </c>
       <c r="E209" s="2">
         <v>42186.0</v>
@@ -4552,7 +4546,7 @@
         <v>2.0275</v>
       </c>
       <c r="D210" s="1">
-        <v>44803.2475</v>
+        <v>1388900.6725</v>
       </c>
       <c r="E210" s="2">
         <v>42186.0</v>
@@ -4572,7 +4566,7 @@
         <v>1.9525</v>
       </c>
       <c r="D211" s="1">
-        <v>8704.865</v>
+        <v>269850.815</v>
       </c>
       <c r="E211" s="2">
         <v>42186.0</v>
@@ -4592,7 +4586,7 @@
         <v>1.094</v>
       </c>
       <c r="D212" s="1">
-        <v>3256778.888</v>
+        <v>1.00960145528E8</v>
       </c>
       <c r="E212" s="2">
         <v>42217.0</v>
@@ -4612,7 +4606,7 @@
         <v>1.108</v>
       </c>
       <c r="D213" s="1">
-        <v>236043.168</v>
+        <v>7317338.208</v>
       </c>
       <c r="E213" s="2">
         <v>42217.0</v>
@@ -4632,7 +4626,7 @@
         <v>1.16</v>
       </c>
       <c r="D214" s="1">
-        <v>324067.094</v>
+        <v>1.0046079914E7</v>
       </c>
       <c r="E214" s="2">
         <v>42217.0</v>
@@ -4652,7 +4646,7 @@
         <v>0.902</v>
       </c>
       <c r="D215" s="1">
-        <v>942293.356</v>
+        <v>2.9211094036E7</v>
       </c>
       <c r="E215" s="2">
         <v>42217.0</v>
@@ -4672,7 +4666,7 @@
         <v>1.188</v>
       </c>
       <c r="D216" s="1">
-        <v>147865.916</v>
+        <v>4583843.396</v>
       </c>
       <c r="E216" s="2">
         <v>42217.0</v>
@@ -4692,7 +4686,7 @@
         <v>1.198</v>
       </c>
       <c r="D217" s="1">
-        <v>127302.07</v>
+        <v>3946364.17</v>
       </c>
       <c r="E217" s="2">
         <v>42217.0</v>
@@ -4712,7 +4706,7 @@
         <v>1.032</v>
       </c>
       <c r="D218" s="1">
-        <v>297145.382</v>
+        <v>9211506.842</v>
       </c>
       <c r="E218" s="2">
         <v>42217.0</v>
@@ -4732,7 +4726,7 @@
         <v>0.96</v>
       </c>
       <c r="D219" s="1">
-        <v>2939839.92</v>
+        <v>9.113503752E7</v>
       </c>
       <c r="E219" s="2">
         <v>42217.0</v>
@@ -4752,7 +4746,7 @@
         <v>1.076</v>
       </c>
       <c r="D220" s="1">
-        <v>77830.876</v>
+        <v>2412757.156</v>
       </c>
       <c r="E220" s="2">
         <v>42217.0</v>
@@ -4772,7 +4766,7 @@
         <v>1.182</v>
       </c>
       <c r="D221" s="1">
-        <v>424509.68</v>
+        <v>1.315980008E7</v>
       </c>
       <c r="E221" s="2">
         <v>42217.0</v>
@@ -4792,7 +4786,7 @@
         <v>1.016</v>
       </c>
       <c r="D222" s="1">
-        <v>165851.338</v>
+        <v>5141391.478</v>
       </c>
       <c r="E222" s="2">
         <v>42217.0</v>
@@ -4812,7 +4806,7 @@
         <v>1.03</v>
       </c>
       <c r="D223" s="1">
-        <v>249832.588</v>
+        <v>7744810.228</v>
       </c>
       <c r="E223" s="2">
         <v>42217.0</v>
@@ -4832,7 +4826,7 @@
         <v>1.14</v>
       </c>
       <c r="D224" s="1">
-        <v>1457532.854</v>
+        <v>4.5183518474E7</v>
       </c>
       <c r="E224" s="2">
         <v>42217.0</v>
@@ -4852,7 +4846,7 @@
         <v>1.158</v>
       </c>
       <c r="D225" s="1">
-        <v>4226923.1</v>
+        <v>1.310346161E8</v>
       </c>
       <c r="E225" s="2">
         <v>42217.0</v>
@@ -4872,7 +4866,7 @@
         <v>1.164</v>
       </c>
       <c r="D226" s="1">
-        <v>432810.868</v>
+        <v>1.3417136908E7</v>
       </c>
       <c r="E226" s="2">
         <v>42217.0</v>
@@ -4892,7 +4886,7 @@
         <v>1.642</v>
       </c>
       <c r="D227" s="1">
-        <v>92419.732</v>
+        <v>2865011.692</v>
       </c>
       <c r="E227" s="2">
         <v>42217.0</v>
@@ -4912,7 +4906,7 @@
         <v>1.792</v>
       </c>
       <c r="D228" s="1">
-        <v>2555.42</v>
+        <v>79218.02</v>
       </c>
       <c r="E228" s="2">
         <v>42217.0</v>
@@ -4932,7 +4926,7 @@
         <v>2.352</v>
       </c>
       <c r="D229" s="1">
-        <v>3415.478</v>
+        <v>105879.818</v>
       </c>
       <c r="E229" s="2">
         <v>42217.0</v>
@@ -4952,7 +4946,7 @@
         <v>1.258</v>
       </c>
       <c r="D230" s="1">
-        <v>11842.424</v>
+        <v>367115.144</v>
       </c>
       <c r="E230" s="2">
         <v>42217.0</v>
@@ -4972,7 +4966,7 @@
         <v>1.712</v>
       </c>
       <c r="D231" s="1">
-        <v>2478.806</v>
+        <v>76842.986</v>
       </c>
       <c r="E231" s="2">
         <v>42217.0</v>
@@ -4992,7 +4986,7 @@
         <v>1.968</v>
       </c>
       <c r="D232" s="1">
-        <v>2633.442</v>
+        <v>81636.702</v>
       </c>
       <c r="E232" s="2">
         <v>42217.0</v>
@@ -5012,7 +5006,7 @@
         <v>1.724</v>
       </c>
       <c r="D233" s="1">
-        <v>8445.252</v>
+        <v>261802.812</v>
       </c>
       <c r="E233" s="2">
         <v>42217.0</v>
@@ -5032,7 +5026,7 @@
         <v>1.578</v>
       </c>
       <c r="D234" s="1">
-        <v>41321.504</v>
+        <v>1280966.624</v>
       </c>
       <c r="E234" s="2">
         <v>42217.0</v>
@@ -5052,7 +5046,7 @@
         <v>1.438</v>
       </c>
       <c r="D235" s="1">
-        <v>2670.166</v>
+        <v>82775.146</v>
       </c>
       <c r="E235" s="2">
         <v>42217.0</v>
@@ -5072,7 +5066,7 @@
         <v>1.498</v>
       </c>
       <c r="D236" s="1">
-        <v>1191.266</v>
+        <v>36929.246</v>
       </c>
       <c r="E236" s="2">
         <v>42217.0</v>
@@ -5092,7 +5086,7 @@
         <v>1.414</v>
       </c>
       <c r="D237" s="1">
-        <v>7519.254</v>
+        <v>233096.874</v>
       </c>
       <c r="E237" s="2">
         <v>42217.0</v>
@@ -5112,7 +5106,7 @@
         <v>1.562</v>
       </c>
       <c r="D238" s="1">
-        <v>2739.562</v>
+        <v>84926.422</v>
       </c>
       <c r="E238" s="2">
         <v>42217.0</v>
@@ -5132,7 +5126,7 @@
         <v>2.184</v>
       </c>
       <c r="D239" s="1">
-        <v>15833.548</v>
+        <v>490839.988</v>
       </c>
       <c r="E239" s="2">
         <v>42217.0</v>
@@ -5152,7 +5146,7 @@
         <v>2.004</v>
       </c>
       <c r="D240" s="1">
-        <v>52584.43</v>
+        <v>1630117.33</v>
       </c>
       <c r="E240" s="2">
         <v>42217.0</v>
@@ -5172,7 +5166,7 @@
         <v>1.928</v>
       </c>
       <c r="D241" s="1">
-        <v>8656.092</v>
+        <v>268338.852</v>
       </c>
       <c r="E241" s="2">
         <v>42217.0</v>
@@ -5192,7 +5186,7 @@
         <v>1.055</v>
       </c>
       <c r="D242" s="1">
-        <v>3227838.9825</v>
+        <v>9.6835169475E7</v>
       </c>
       <c r="E242" s="2">
         <v>42248.0</v>
@@ -5212,7 +5206,7 @@
         <v>1.145</v>
       </c>
       <c r="D243" s="1">
-        <v>215257.9175</v>
+        <v>6457737.525</v>
       </c>
       <c r="E243" s="2">
         <v>42248.0</v>
@@ -5232,7 +5226,7 @@
         <v>1.23</v>
       </c>
       <c r="D244" s="1">
-        <v>277776.6925</v>
+        <v>8333300.775</v>
       </c>
       <c r="E244" s="2">
         <v>42248.0</v>
@@ -5252,7 +5246,7 @@
         <v>0.8675</v>
       </c>
       <c r="D245" s="1">
-        <v>1030624.95</v>
+        <v>3.09187485E7</v>
       </c>
       <c r="E245" s="2">
         <v>42248.0</v>
@@ -5272,7 +5266,7 @@
         <v>0.9825</v>
       </c>
       <c r="D246" s="1">
-        <v>170920.4925</v>
+        <v>5127614.775</v>
       </c>
       <c r="E246" s="2">
         <v>42248.0</v>
@@ -5292,7 +5286,7 @@
         <v>1.12</v>
       </c>
       <c r="D247" s="1">
-        <v>133180.655</v>
+        <v>3995419.65</v>
       </c>
       <c r="E247" s="2">
         <v>42248.0</v>
@@ -5312,7 +5306,7 @@
         <v>0.96</v>
       </c>
       <c r="D248" s="1">
-        <v>303822.93</v>
+        <v>9114687.9</v>
       </c>
       <c r="E248" s="2">
         <v>42248.0</v>
@@ -5332,7 +5326,7 @@
         <v>0.9475</v>
       </c>
       <c r="D249" s="1">
-        <v>2649945.82</v>
+        <v>7.94983746E7</v>
       </c>
       <c r="E249" s="2">
         <v>42248.0</v>
@@ -5352,7 +5346,7 @@
         <v>1.0475</v>
       </c>
       <c r="D250" s="1">
-        <v>79029.735</v>
+        <v>2370892.05</v>
       </c>
       <c r="E250" s="2">
         <v>42248.0</v>
@@ -5372,7 +5366,7 @@
         <v>1.1325</v>
       </c>
       <c r="D251" s="1">
-        <v>461567.78</v>
+        <v>1.38470334E7</v>
       </c>
       <c r="E251" s="2">
         <v>42248.0</v>
@@ -5392,7 +5386,7 @@
         <v>1.0025</v>
       </c>
       <c r="D252" s="1">
-        <v>172199.125</v>
+        <v>5165973.75</v>
       </c>
       <c r="E252" s="2">
         <v>42248.0</v>
@@ -5412,7 +5406,7 @@
         <v>1.0175</v>
       </c>
       <c r="D253" s="1">
-        <v>223014.175</v>
+        <v>6690425.25</v>
       </c>
       <c r="E253" s="2">
         <v>42248.0</v>
@@ -5432,7 +5426,7 @@
         <v>1.18</v>
       </c>
       <c r="D254" s="1">
-        <v>1303384.3375</v>
+        <v>3.9101530125E7</v>
       </c>
       <c r="E254" s="2">
         <v>42248.0</v>
@@ -5452,7 +5446,7 @@
         <v>1.165</v>
       </c>
       <c r="D255" s="1">
-        <v>3841755.2475</v>
+        <v>1.15252657425E8</v>
       </c>
       <c r="E255" s="2">
         <v>42248.0</v>
@@ -5472,7 +5466,7 @@
         <v>1.0625</v>
       </c>
       <c r="D256" s="1">
-        <v>411411.3925</v>
+        <v>1.2342341775E7</v>
       </c>
       <c r="E256" s="2">
         <v>42248.0</v>
@@ -5492,7 +5486,7 @@
         <v>1.655</v>
       </c>
       <c r="D257" s="1">
-        <v>81394.5625</v>
+        <v>2441836.875</v>
       </c>
       <c r="E257" s="2">
         <v>42248.0</v>
@@ -5512,7 +5506,7 @@
         <v>1.925</v>
       </c>
       <c r="D258" s="1">
-        <v>2078.9025</v>
+        <v>62367.075</v>
       </c>
       <c r="E258" s="2">
         <v>42248.0</v>
@@ -5532,7 +5526,7 @@
         <v>2.3625</v>
       </c>
       <c r="D259" s="1">
-        <v>3546.73</v>
+        <v>106401.9</v>
       </c>
       <c r="E259" s="2">
         <v>42248.0</v>
@@ -5552,7 +5546,7 @@
         <v>1.4275</v>
       </c>
       <c r="D260" s="1">
-        <v>11845.6775</v>
+        <v>355370.325</v>
       </c>
       <c r="E260" s="2">
         <v>42248.0</v>
@@ -5572,7 +5566,7 @@
         <v>1.655</v>
       </c>
       <c r="D261" s="1">
-        <v>2245.105</v>
+        <v>67353.15</v>
       </c>
       <c r="E261" s="2">
         <v>42248.0</v>
@@ -5592,7 +5586,7 @@
         <v>2.1675</v>
       </c>
       <c r="D262" s="1">
-        <v>1722.2475</v>
+        <v>51667.425</v>
       </c>
       <c r="E262" s="2">
         <v>42248.0</v>
@@ -5612,7 +5606,7 @@
         <v>2.1825</v>
       </c>
       <c r="D263" s="1">
-        <v>4919.3025</v>
+        <v>147579.075</v>
       </c>
       <c r="E263" s="2">
         <v>42248.0</v>
@@ -5632,7 +5626,7 @@
         <v>1.585</v>
       </c>
       <c r="D264" s="1">
-        <v>41964.6025</v>
+        <v>1258938.075</v>
       </c>
       <c r="E264" s="2">
         <v>42248.0</v>
@@ -5652,7 +5646,7 @@
         <v>1.6275</v>
       </c>
       <c r="D265" s="1">
-        <v>1971.5225</v>
+        <v>59145.675</v>
       </c>
       <c r="E265" s="2">
         <v>42248.0</v>
@@ -5672,7 +5666,7 @@
         <v>1.4675</v>
       </c>
       <c r="D266" s="1">
-        <v>1408.49</v>
+        <v>42254.7</v>
       </c>
       <c r="E266" s="2">
         <v>42248.0</v>
@@ -5692,7 +5686,7 @@
         <v>1.57</v>
       </c>
       <c r="D267" s="1">
-        <v>5875.375</v>
+        <v>176261.25</v>
       </c>
       <c r="E267" s="2">
         <v>42248.0</v>
@@ -5712,7 +5706,7 @@
         <v>1.635</v>
       </c>
       <c r="D268" s="1">
-        <v>2197.6175</v>
+        <v>65928.525</v>
       </c>
       <c r="E268" s="2">
         <v>42248.0</v>
@@ -5732,7 +5726,7 @@
         <v>2.105</v>
       </c>
       <c r="D269" s="1">
-        <v>17233.6275</v>
+        <v>517008.825</v>
       </c>
       <c r="E269" s="2">
         <v>42248.0</v>
@@ -5752,7 +5746,7 @@
         <v>1.97</v>
       </c>
       <c r="D270" s="1">
-        <v>50843.575</v>
+        <v>1525307.25</v>
       </c>
       <c r="E270" s="2">
         <v>42248.0</v>
@@ -5772,7 +5766,7 @@
         <v>1.9425</v>
       </c>
       <c r="D271" s="1">
-        <v>6644.01</v>
+        <v>199320.3</v>
       </c>
       <c r="E271" s="2">
         <v>42248.0</v>
@@ -5792,7 +5786,7 @@
         <v>1.05</v>
       </c>
       <c r="D272" s="1">
-        <v>2867974.55</v>
+        <v>8.890721105E7</v>
       </c>
       <c r="E272" s="4">
         <v>42278.0</v>
@@ -5812,7 +5806,7 @@
         <v>1.0625</v>
       </c>
       <c r="D273" s="1">
-        <v>215254.1825</v>
+        <v>6672879.6575</v>
       </c>
       <c r="E273" s="4">
         <v>42278.0</v>
@@ -5832,7 +5826,7 @@
         <v>1.2025</v>
       </c>
       <c r="D274" s="1">
-        <v>292273.505</v>
+        <v>9060478.655</v>
       </c>
       <c r="E274" s="4">
         <v>42278.0</v>
@@ -5852,7 +5846,7 @@
         <v>0.8475</v>
       </c>
       <c r="D275" s="1">
-        <v>959247.55</v>
+        <v>2.973667405E7</v>
       </c>
       <c r="E275" s="4">
         <v>42278.0</v>
@@ -5872,7 +5866,7 @@
         <v>1.0175</v>
       </c>
       <c r="D276" s="1">
-        <v>144887.4875</v>
+        <v>4491512.1125</v>
       </c>
       <c r="E276" s="4">
         <v>42278.0</v>
@@ -5892,7 +5886,7 @@
         <v>1.1125</v>
       </c>
       <c r="D277" s="1">
-        <v>121429.6425</v>
+        <v>3764318.9175</v>
       </c>
       <c r="E277" s="4">
         <v>42278.0</v>
@@ -5912,7 +5906,7 @@
         <v>0.95</v>
       </c>
       <c r="D278" s="1">
-        <v>265578.165</v>
+        <v>8232923.115</v>
       </c>
       <c r="E278" s="4">
         <v>42278.0</v>
@@ -5932,7 +5926,7 @@
         <v>0.935</v>
       </c>
       <c r="D279" s="1">
-        <v>2464897.605</v>
+        <v>7.6411825755E7</v>
       </c>
       <c r="E279" s="4">
         <v>42278.0</v>
@@ -5952,7 +5946,7 @@
         <v>1.0575</v>
       </c>
       <c r="D280" s="1">
-        <v>69097.26</v>
+        <v>2142015.06</v>
       </c>
       <c r="E280" s="4">
         <v>42278.0</v>
@@ -5972,7 +5966,7 @@
         <v>1.12</v>
       </c>
       <c r="D281" s="1">
-        <v>437439.5725</v>
+        <v>1.35606267475E7</v>
       </c>
       <c r="E281" s="4">
         <v>42278.0</v>
@@ -5992,7 +5986,7 @@
         <v>0.935</v>
       </c>
       <c r="D282" s="1">
-        <v>164113.4625</v>
+        <v>5087517.3375</v>
       </c>
       <c r="E282" s="4">
         <v>42278.0</v>
@@ -6012,7 +6006,7 @@
         <v>1.0075</v>
       </c>
       <c r="D283" s="1">
-        <v>209502.32</v>
+        <v>6494571.92</v>
       </c>
       <c r="E283" s="4">
         <v>42278.0</v>
@@ -6032,7 +6026,7 @@
         <v>1.185</v>
       </c>
       <c r="D284" s="1">
-        <v>1336657.5475</v>
+        <v>4.14363839725E7</v>
       </c>
       <c r="E284" s="4">
         <v>42278.0</v>
@@ -6052,7 +6046,7 @@
         <v>1.145</v>
       </c>
       <c r="D285" s="1">
-        <v>3766558.3175</v>
+        <v>1.167633078425E8</v>
       </c>
       <c r="E285" s="4">
         <v>42278.0</v>
@@ -6072,7 +6066,7 @@
         <v>1.0975</v>
       </c>
       <c r="D286" s="1">
-        <v>323260.7125</v>
+        <v>1.00210820875E7</v>
       </c>
       <c r="E286" s="4">
         <v>42278.0</v>
@@ -6092,9 +6086,9 @@
         <v>1.6125</v>
       </c>
       <c r="D287" s="1">
-        <v>73158.6075</v>
-      </c>
-      <c r="E287" s="5">
+        <v>2267916.8325</v>
+      </c>
+      <c r="E287" s="4">
         <v>42278.0</v>
       </c>
       <c r="F287" s="1" t="s">
@@ -6112,9 +6106,9 @@
         <v>1.695</v>
       </c>
       <c r="D288" s="1">
-        <v>2055.9875</v>
-      </c>
-      <c r="E288" s="5">
+        <v>63735.6125</v>
+      </c>
+      <c r="E288" s="4">
         <v>42278.0</v>
       </c>
       <c r="F288" s="1" t="s">
@@ -6132,9 +6126,9 @@
         <v>2.1825</v>
       </c>
       <c r="D289" s="1">
-        <v>2995.0525</v>
-      </c>
-      <c r="E289" s="5">
+        <v>92846.6275</v>
+      </c>
+      <c r="E289" s="4">
         <v>42278.0</v>
       </c>
       <c r="F289" s="1" t="s">
@@ -6152,9 +6146,9 @@
         <v>1.48</v>
       </c>
       <c r="D290" s="1">
-        <v>10893.06</v>
-      </c>
-      <c r="E290" s="5">
+        <v>337684.86</v>
+      </c>
+      <c r="E290" s="4">
         <v>42278.0</v>
       </c>
       <c r="F290" s="1" t="s">
@@ -6172,9 +6166,9 @@
         <v>1.5025</v>
       </c>
       <c r="D291" s="1">
-        <v>2183.9525</v>
-      </c>
-      <c r="E291" s="5">
+        <v>67702.5275</v>
+      </c>
+      <c r="E291" s="4">
         <v>42278.0</v>
       </c>
       <c r="F291" s="1" t="s">
@@ -6192,9 +6186,9 @@
         <v>2.1</v>
       </c>
       <c r="D292" s="1">
-        <v>2167.8175</v>
-      </c>
-      <c r="E292" s="5">
+        <v>67202.3425</v>
+      </c>
+      <c r="E292" s="4">
         <v>42278.0</v>
       </c>
       <c r="F292" s="1" t="s">
@@ -6212,9 +6206,9 @@
         <v>2.225</v>
       </c>
       <c r="D293" s="1">
-        <v>4413.2575</v>
-      </c>
-      <c r="E293" s="5">
+        <v>136810.9825</v>
+      </c>
+      <c r="E293" s="4">
         <v>42278.0</v>
       </c>
       <c r="F293" s="1" t="s">
@@ -6232,9 +6226,9 @@
         <v>1.6075</v>
       </c>
       <c r="D294" s="1">
-        <v>36260.7475</v>
-      </c>
-      <c r="E294" s="5">
+        <v>1124083.1725</v>
+      </c>
+      <c r="E294" s="4">
         <v>42278.0</v>
       </c>
       <c r="F294" s="1" t="s">
@@ -6252,9 +6246,9 @@
         <v>1.67</v>
       </c>
       <c r="D295" s="1">
-        <v>1468.6825</v>
-      </c>
-      <c r="E295" s="5">
+        <v>45529.1575</v>
+      </c>
+      <c r="E295" s="4">
         <v>42278.0</v>
       </c>
       <c r="F295" s="1" t="s">
@@ -6272,9 +6266,9 @@
         <v>1.505</v>
       </c>
       <c r="D296" s="1">
-        <v>1437.6675</v>
-      </c>
-      <c r="E296" s="5">
+        <v>44567.6925</v>
+      </c>
+      <c r="E296" s="4">
         <v>42278.0</v>
       </c>
       <c r="F296" s="1" t="s">
@@ -6292,9 +6286,9 @@
         <v>1.6625</v>
       </c>
       <c r="D297" s="1">
-        <v>4956.3125</v>
-      </c>
-      <c r="E297" s="5">
+        <v>153645.6875</v>
+      </c>
+      <c r="E297" s="4">
         <v>42278.0</v>
       </c>
       <c r="F297" s="1" t="s">
@@ -6312,9 +6306,9 @@
         <v>1.53</v>
       </c>
       <c r="D298" s="1">
-        <v>3160.3225</v>
-      </c>
-      <c r="E298" s="5">
+        <v>97969.9975</v>
+      </c>
+      <c r="E298" s="4">
         <v>42278.0</v>
       </c>
       <c r="F298" s="1" t="s">
@@ -6332,9 +6326,9 @@
         <v>2.0875</v>
       </c>
       <c r="D299" s="1">
-        <v>14158.8175</v>
-      </c>
-      <c r="E299" s="5">
+        <v>438923.3425</v>
+      </c>
+      <c r="E299" s="4">
         <v>42278.0</v>
       </c>
       <c r="F299" s="1" t="s">
@@ -6352,9 +6346,9 @@
         <v>1.725</v>
       </c>
       <c r="D300" s="1">
-        <v>54161.545</v>
-      </c>
-      <c r="E300" s="5">
+        <v>1679007.895</v>
+      </c>
+      <c r="E300" s="4">
         <v>42278.0</v>
       </c>
       <c r="F300" s="1" t="s">
@@ -6372,7 +6366,7 @@
         <v>1.6175</v>
       </c>
       <c r="D301" s="1">
-        <v>8384.74</v>
+        <v>259926.94</v>
       </c>
       <c r="E301" s="4">
         <v>42278.0</v>
@@ -6392,7 +6386,7 @@
         <v>1.034</v>
       </c>
       <c r="D302" s="1">
-        <v>2741669.248</v>
+        <v>8.225007744E7</v>
       </c>
       <c r="E302" s="4">
         <v>42309.0</v>
@@ -6412,7 +6406,7 @@
         <v>1.128</v>
       </c>
       <c r="D303" s="1">
-        <v>186682.676</v>
+        <v>5600480.28</v>
       </c>
       <c r="E303" s="4">
         <v>42309.0</v>
@@ -6432,7 +6426,7 @@
         <v>1.206</v>
       </c>
       <c r="D304" s="1">
-        <v>267238.748</v>
+        <v>8017162.44</v>
       </c>
       <c r="E304" s="4">
         <v>42309.0</v>
@@ -6452,7 +6446,7 @@
         <v>0.752</v>
       </c>
       <c r="D305" s="1">
-        <v>937349.262</v>
+        <v>2.812047786E7</v>
       </c>
       <c r="E305" s="4">
         <v>42309.0</v>
@@ -6472,7 +6466,7 @@
         <v>1.048</v>
       </c>
       <c r="D306" s="1">
-        <v>128661.35</v>
+        <v>3859840.5</v>
       </c>
       <c r="E306" s="4">
         <v>42309.0</v>
@@ -6492,7 +6486,7 @@
         <v>1.082</v>
       </c>
       <c r="D307" s="1">
-        <v>116918.358</v>
+        <v>3507550.74</v>
       </c>
       <c r="E307" s="4">
         <v>42309.0</v>
@@ -6512,7 +6506,7 @@
         <v>0.958</v>
       </c>
       <c r="D308" s="1">
-        <v>227383.976</v>
+        <v>6821519.28</v>
       </c>
       <c r="E308" s="4">
         <v>42309.0</v>
@@ -6532,7 +6526,7 @@
         <v>0.822</v>
       </c>
       <c r="D309" s="1">
-        <v>2498266.434</v>
+        <v>7.494799302E7</v>
       </c>
       <c r="E309" s="4">
         <v>42309.0</v>
@@ -6552,7 +6546,7 @@
         <v>0.968</v>
       </c>
       <c r="D310" s="1">
-        <v>73830.772</v>
+        <v>2214923.16</v>
       </c>
       <c r="E310" s="4">
         <v>42309.0</v>
@@ -6572,7 +6566,7 @@
         <v>1.076</v>
       </c>
       <c r="D311" s="1">
-        <v>446741.312</v>
+        <v>1.340223936E7</v>
       </c>
       <c r="E311" s="4">
         <v>42309.0</v>
@@ -6592,7 +6586,7 @@
         <v>0.984</v>
       </c>
       <c r="D312" s="1">
-        <v>133316.212</v>
+        <v>3999486.36</v>
       </c>
       <c r="E312" s="4">
         <v>42309.0</v>
@@ -6612,7 +6606,7 @@
         <v>0.95</v>
       </c>
       <c r="D313" s="1">
-        <v>193228.118</v>
+        <v>5796843.54</v>
       </c>
       <c r="E313" s="4">
         <v>42309.0</v>
@@ -6632,7 +6626,7 @@
         <v>1.106</v>
       </c>
       <c r="D314" s="1">
-        <v>1411029.696</v>
+        <v>4.233089088E7</v>
       </c>
       <c r="E314" s="4">
         <v>42309.0</v>
@@ -6652,7 +6646,7 @@
         <v>1.132</v>
       </c>
       <c r="D315" s="1">
-        <v>3633268.098</v>
+        <v>1.0899804294E8</v>
       </c>
       <c r="E315" s="4">
         <v>42309.0</v>
@@ -6672,7 +6666,7 @@
         <v>1.086</v>
       </c>
       <c r="D316" s="1">
-        <v>324103.082</v>
+        <v>9723092.46</v>
       </c>
       <c r="E316" s="4">
         <v>42309.0</v>
@@ -6692,7 +6686,7 @@
         <v>1.57</v>
       </c>
       <c r="D317" s="1">
-        <v>70437.106</v>
+        <v>2113113.18</v>
       </c>
       <c r="E317" s="4">
         <v>42309.0</v>
@@ -6712,7 +6706,7 @@
         <v>1.76</v>
       </c>
       <c r="D318" s="1">
-        <v>1735.99</v>
+        <v>52079.7</v>
       </c>
       <c r="E318" s="4">
         <v>42309.0</v>
@@ -6732,7 +6726,7 @@
         <v>2.194</v>
       </c>
       <c r="D319" s="1">
-        <v>2687.234</v>
+        <v>80617.02</v>
       </c>
       <c r="E319" s="4">
         <v>42309.0</v>
@@ -6752,7 +6746,7 @@
         <v>1.488</v>
       </c>
       <c r="D320" s="1">
-        <v>8972.616</v>
+        <v>269178.48</v>
       </c>
       <c r="E320" s="4">
         <v>42309.0</v>
@@ -6772,7 +6766,7 @@
         <v>1.55</v>
       </c>
       <c r="D321" s="1">
-        <v>1687.094</v>
+        <v>50612.82</v>
       </c>
       <c r="E321" s="4">
         <v>42309.0</v>
@@ -6792,7 +6786,7 @@
         <v>1.86</v>
       </c>
       <c r="D322" s="1">
-        <v>1750.596</v>
+        <v>52517.88</v>
       </c>
       <c r="E322" s="4">
         <v>42309.0</v>
@@ -6812,7 +6806,7 @@
         <v>2.018</v>
       </c>
       <c r="D323" s="1">
-        <v>4862.52</v>
+        <v>145875.6</v>
       </c>
       <c r="E323" s="4">
         <v>42309.0</v>
@@ -6832,7 +6826,7 @@
         <v>1.352</v>
       </c>
       <c r="D324" s="1">
-        <v>47867.748</v>
+        <v>1436032.44</v>
       </c>
       <c r="E324" s="4">
         <v>42309.0</v>
@@ -6852,7 +6846,7 @@
         <v>1.644</v>
       </c>
       <c r="D325" s="1">
-        <v>1255.698</v>
+        <v>37670.94</v>
       </c>
       <c r="E325" s="4">
         <v>42309.0</v>
@@ -6872,7 +6866,7 @@
         <v>1.43</v>
       </c>
       <c r="D326" s="1">
-        <v>1321.836</v>
+        <v>39655.08</v>
       </c>
       <c r="E326" s="4">
         <v>42309.0</v>
@@ -6892,7 +6886,7 @@
         <v>1.548</v>
       </c>
       <c r="D327" s="1">
-        <v>4932.274</v>
+        <v>147968.22</v>
       </c>
       <c r="E327" s="4">
         <v>42309.0</v>
@@ -6912,12 +6906,12 @@
         <v>1.634</v>
       </c>
       <c r="D328" s="1">
-        <v>2074.732</v>
+        <v>62241.96</v>
       </c>
       <c r="E328" s="4">
         <v>42309.0</v>
       </c>
-      <c r="F328" s="1" t="s">
+      <c r="F328" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6932,12 +6926,12 @@
         <v>1.88</v>
       </c>
       <c r="D329" s="1">
-        <v>12676.4</v>
+        <v>380292.0</v>
       </c>
       <c r="E329" s="4">
         <v>42309.0</v>
       </c>
-      <c r="F329" s="1" t="s">
+      <c r="F329" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6952,12 +6946,12 @@
         <v>1.634</v>
       </c>
       <c r="D330" s="1">
-        <v>52022.012</v>
+        <v>1560660.36</v>
       </c>
       <c r="E330" s="4">
         <v>42309.0</v>
       </c>
-      <c r="F330" s="1" t="s">
+      <c r="F330" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6972,12 +6966,12 @@
         <v>1.612</v>
       </c>
       <c r="D331" s="1">
-        <v>8863.476</v>
+        <v>265904.28</v>
       </c>
       <c r="E331" s="4">
         <v>42309.0</v>
       </c>
-      <c r="F331" s="1" t="s">
+      <c r="F331" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6992,12 +6986,12 @@
         <v>1.0125</v>
       </c>
       <c r="D332" s="1">
-        <v>2668785.9175</v>
+        <v>8.27323634425E7</v>
       </c>
       <c r="E332" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F332" s="1" t="s">
+      <c r="F332" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7012,12 +7006,12 @@
         <v>1.1275</v>
       </c>
       <c r="D333" s="1">
-        <v>178021.5475</v>
+        <v>5518667.9725</v>
       </c>
       <c r="E333" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F333" s="1" t="s">
+      <c r="F333" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7032,12 +7026,12 @@
         <v>1.22</v>
       </c>
       <c r="D334" s="1">
-        <v>246553.9725</v>
+        <v>7643173.1475</v>
       </c>
       <c r="E334" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F334" s="1" t="s">
+      <c r="F334" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7052,12 +7046,12 @@
         <v>0.75</v>
       </c>
       <c r="D335" s="1">
-        <v>963823.0025</v>
+        <v>2.98785130775E7</v>
       </c>
       <c r="E335" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F335" s="1" t="s">
+      <c r="F335" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7072,12 +7066,12 @@
         <v>1.0225</v>
       </c>
       <c r="D336" s="1">
-        <v>127633.275</v>
+        <v>3956631.525</v>
       </c>
       <c r="E336" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F336" s="1" t="s">
+      <c r="F336" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7092,12 +7086,12 @@
         <v>1.0825</v>
       </c>
       <c r="D337" s="1">
-        <v>115572.9475</v>
+        <v>3582761.3725</v>
       </c>
       <c r="E337" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F337" s="1" t="s">
+      <c r="F337" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7112,12 +7106,12 @@
         <v>0.9075</v>
       </c>
       <c r="D338" s="1">
-        <v>246286.5075</v>
+        <v>7634881.7325</v>
       </c>
       <c r="E338" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F338" s="1" t="s">
+      <c r="F338" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7132,12 +7126,12 @@
         <v>0.7625</v>
       </c>
       <c r="D339" s="1">
-        <v>2553850.2975</v>
+        <v>7.91693592225E7</v>
       </c>
       <c r="E339" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F339" s="1" t="s">
+      <c r="F339" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7152,9 +7146,9 @@
         <v>0.9575</v>
       </c>
       <c r="D340" s="1">
-        <v>74479.885</v>
-      </c>
-      <c r="E340" s="4">
+        <v>2308876.435</v>
+      </c>
+      <c r="E340" s="5">
         <v>42339.0</v>
       </c>
       <c r="F340" s="1" t="s">
@@ -7172,7 +7166,7 @@
         <v>1.105</v>
       </c>
       <c r="D341" s="1">
-        <v>441357.38</v>
+        <v>1.368207878E7</v>
       </c>
       <c r="E341" s="4">
         <v>42339.0</v>
@@ -7192,7 +7186,7 @@
         <v>0.965</v>
       </c>
       <c r="D342" s="1">
-        <v>133864.655</v>
+        <v>4149804.305</v>
       </c>
       <c r="E342" s="4">
         <v>42339.0</v>
@@ -7212,7 +7206,7 @@
         <v>0.9075</v>
       </c>
       <c r="D343" s="1">
-        <v>192303.4275</v>
+        <v>5961406.2525</v>
       </c>
       <c r="E343" s="4">
         <v>42339.0</v>
@@ -7232,7 +7226,7 @@
         <v>1.18</v>
       </c>
       <c r="D344" s="1">
-        <v>1148250.215</v>
+        <v>3.5595756665E7</v>
       </c>
       <c r="E344" s="4">
         <v>42339.0</v>
@@ -7252,7 +7246,7 @@
         <v>1.1575</v>
       </c>
       <c r="D345" s="1">
-        <v>3315381.5775</v>
+        <v>1.027768289025E8</v>
       </c>
       <c r="E345" s="4">
         <v>42339.0</v>
@@ -7272,7 +7266,7 @@
         <v>1.11</v>
       </c>
       <c r="D346" s="1">
-        <v>324986.94</v>
+        <v>1.007459514E7</v>
       </c>
       <c r="E346" s="4">
         <v>42339.0</v>
@@ -7292,12 +7286,12 @@
         <v>1.5425</v>
       </c>
       <c r="D347" s="1">
-        <v>66572.3525</v>
+        <v>2063742.9275</v>
       </c>
       <c r="E347" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F347" s="6" t="s">
+      <c r="F347" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7312,12 +7306,12 @@
         <v>1.71</v>
       </c>
       <c r="D348" s="1">
-        <v>4450.3025</v>
+        <v>137959.3775</v>
       </c>
       <c r="E348" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F348" s="6" t="s">
+      <c r="F348" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7332,12 +7326,12 @@
         <v>2.265</v>
       </c>
       <c r="D349" s="1">
-        <v>4797.0225</v>
+        <v>148707.6975</v>
       </c>
       <c r="E349" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F349" s="7" t="s">
+      <c r="F349" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7352,12 +7346,12 @@
         <v>1.355</v>
       </c>
       <c r="D350" s="1">
-        <v>9890.8525</v>
+        <v>306616.4275</v>
       </c>
       <c r="E350" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F350" s="7" t="s">
+      <c r="F350" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7372,12 +7366,12 @@
         <v>1.44</v>
       </c>
       <c r="D351" s="1">
-        <v>1875.695</v>
+        <v>58146.545</v>
       </c>
       <c r="E351" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F351" s="7" t="s">
+      <c r="F351" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7392,12 +7386,12 @@
         <v>1.8275</v>
       </c>
       <c r="D352" s="1">
-        <v>1764.3075</v>
+        <v>54693.5325</v>
       </c>
       <c r="E352" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F352" s="7" t="s">
+      <c r="F352" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7412,12 +7406,12 @@
         <v>1.9475</v>
       </c>
       <c r="D353" s="1">
-        <v>4895.6625</v>
+        <v>151765.5375</v>
       </c>
       <c r="E353" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F353" s="7" t="s">
+      <c r="F353" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7432,12 +7426,12 @@
         <v>1.1725</v>
       </c>
       <c r="D354" s="1">
-        <v>50154.415</v>
+        <v>1554786.865</v>
       </c>
       <c r="E354" s="4">
         <v>42339.0</v>
       </c>
-      <c r="F354" s="7" t="s">
+      <c r="F354" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7452,12 +7446,12 @@
         <v>1.5825</v>
       </c>
       <c r="D355" s="1">
-        <v>1072.55</v>
-      </c>
-      <c r="E355" s="4">
+        <v>33249.05</v>
+      </c>
+      <c r="E355" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F355" s="7" t="s">
+      <c r="F355" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7472,12 +7466,12 @@
         <v>1.515</v>
       </c>
       <c r="D356" s="1">
-        <v>1284.78</v>
-      </c>
-      <c r="E356" s="4">
+        <v>39828.18</v>
+      </c>
+      <c r="E356" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F356" s="7" t="s">
+      <c r="F356" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7492,12 +7486,12 @@
         <v>1.575</v>
       </c>
       <c r="D357" s="1">
-        <v>4114.995</v>
-      </c>
-      <c r="E357" s="4">
+        <v>127564.845</v>
+      </c>
+      <c r="E357" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F357" s="7" t="s">
+      <c r="F357" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7512,12 +7506,12 @@
         <v>1.54</v>
       </c>
       <c r="D358" s="1">
-        <v>1944.6675</v>
-      </c>
-      <c r="E358" s="4">
+        <v>60284.6925</v>
+      </c>
+      <c r="E358" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F358" s="7" t="s">
+      <c r="F358" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7532,12 +7526,12 @@
         <v>1.845</v>
       </c>
       <c r="D359" s="1">
-        <v>22134.0925</v>
-      </c>
-      <c r="E359" s="4">
+        <v>686156.8675</v>
+      </c>
+      <c r="E359" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F359" s="7" t="s">
+      <c r="F359" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7552,12 +7546,12 @@
         <v>1.7</v>
       </c>
       <c r="D360" s="1">
-        <v>73355.8</v>
-      </c>
-      <c r="E360" s="4">
+        <v>2274029.8</v>
+      </c>
+      <c r="E360" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F360" s="7" t="s">
+      <c r="F360" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7572,59 +7566,14 @@
         <v>1.6325</v>
       </c>
       <c r="D361" s="1">
-        <v>8672.7925</v>
-      </c>
-      <c r="E361" s="4">
+        <v>268856.5675</v>
+      </c>
+      <c r="E361" s="5">
         <v>42339.0</v>
       </c>
-      <c r="F361" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="363">
-      <c r="E363" s="5"/>
-    </row>
-    <row r="364">
-      <c r="E364" s="5"/>
-    </row>
-    <row r="365">
-      <c r="E365" s="5"/>
-    </row>
-    <row r="366">
-      <c r="E366" s="5"/>
-    </row>
-    <row r="367">
-      <c r="E367" s="5"/>
-    </row>
-    <row r="368">
-      <c r="E368" s="5"/>
-    </row>
-    <row r="369">
-      <c r="E369" s="5"/>
-    </row>
-    <row r="370">
-      <c r="E370" s="5"/>
-    </row>
-    <row r="371">
-      <c r="E371" s="5"/>
-    </row>
-    <row r="372">
-      <c r="E372" s="5"/>
-    </row>
-    <row r="373">
-      <c r="E373" s="5"/>
-    </row>
-    <row r="374">
-      <c r="E374" s="5"/>
-    </row>
-    <row r="375">
-      <c r="E375" s="5"/>
-    </row>
-    <row r="376">
-      <c r="E376" s="5"/>
-    </row>
-    <row r="377">
-      <c r="E377" s="5"/>
+      <c r="F361" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>